<commit_message>
back and forth from castle done and npc collision without dialogue
</commit_message>
<xml_diff>
--- a/data/non_player_characters.xlsx
+++ b/data/non_player_characters.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\Python\Kolo_game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\Backup\Kolo_game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7ADDF0D-4C69-4385-976E-D91976D87A29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -41,16 +42,16 @@
     <t>sprite</t>
   </si>
   <si>
-    <t>pingu.png</t>
-  </si>
-  <si>
-    <t>first_map</t>
+    <t>second_map</t>
+  </si>
+  <si>
+    <t>SNORLAX.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,19 +363,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,21 +393,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>111</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>512</v>
+      </c>
+      <c r="D2">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
my bad... now is full automation
</commit_message>
<xml_diff>
--- a/data/non_player_characters.xlsx
+++ b/data/non_player_characters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\Backup\Kolo_game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7ADDF0D-4C69-4385-976E-D91976D87A29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1615FFB0-DFD3-471E-A383-60A9A7310CE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>npc_id</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>SNORLAX.png</t>
+  </si>
+  <si>
+    <t>castle</t>
+  </si>
+  <si>
+    <t>MIME.png</t>
   </si>
 </sst>
 </file>
@@ -364,15 +370,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -410,6 +417,23 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>222</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>256</v>
+      </c>
+      <c r="D3">
+        <v>896</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
example of a fight completed
</commit_message>
<xml_diff>
--- a/data/non_player_characters.xlsx
+++ b/data/non_player_characters.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\Kolo_game\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9B94A2-C95C-40B1-868B-85692D116057}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="20460" windowHeight="9705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>npc_id</t>
   </si>
@@ -64,13 +70,19 @@
   </si>
   <si>
     <t>arm</t>
+  </si>
+  <si>
+    <t>BLASTOISE.png</t>
+  </si>
+  <si>
+    <t>Blastoise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,28 +386,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>111</v>
       </c>
@@ -453,7 +465,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>222</v>
       </c>
@@ -482,27 +494,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>333</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>130</v>
+        <v>320</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G4">
-        <v>375</v>
+        <v>50</v>
       </c>
       <c r="H4">
         <v>31</v>

</xml_diff>